<commit_message>
fix: real-world usage figure
</commit_message>
<xml_diff>
--- a/outputs/metadata_elements_count.xlsx
+++ b/outputs/metadata_elements_count.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H140"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Description of the dataset sharing method</t>
+          <t>Description of the intended use of the dataset</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Description of the intended use of the dataset</t>
+          <t>Description of the dataset update plan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Description of the data collection process</t>
+          <t>Description of the dataset sharing method</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dataset publication date</t>
+          <t>Description of the data collection process</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Information about the owners of the dataset</t>
+          <t>Details about the funding of the dataset</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -678,7 +678,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Description of the dataset update plan</t>
+          <t>Information about the owners of the dataset</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Details about the funding of the dataset</t>
+          <t>Dataset publication date</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -798,7 +798,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Description of the data collection timeframe</t>
+          <t>Description of the instances included in the dataset</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -838,12 +838,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Information about the maintainers of the dataset</t>
+          <t>Description of the dataset</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -878,7 +878,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DOI or link of the dataset</t>
+          <t>Information about the maintainers of the dataset</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -903,7 +903,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -958,7 +958,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Description of the dataset license and/or terms of use</t>
+          <t>DOI or link of the dataset</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -998,7 +998,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Description of the instances included in the dataset</t>
+          <t>Description of the data labeling process</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Description of the purpose for creating the dataset</t>
+          <t>Description and handling of the missing data</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1078,17 +1078,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Description of the dataset</t>
+          <t>Description of the purpose for creating the dataset</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Description of the restrictions on the usage of the data</t>
+          <t>Description of the dataset license and/or terms of use</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1158,7 +1158,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Description of the data labeling process</t>
+          <t>Description of the sensitive data</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1198,7 +1198,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Description and handling of the missing data</t>
+          <t>Description of the data collection timeframe</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1238,7 +1238,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Description of the sensitive data</t>
+          <t>Description of the restrictions on the usage of the data</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1278,7 +1278,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Details of the data modalities</t>
+          <t>Version of the dataset associated with this dataset documentation</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1288,12 +1288,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1318,7 +1318,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Information about the creators of the dataset</t>
+          <t>Description of the data sampling process</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1358,7 +1358,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Description of the upsetting data</t>
+          <t>Description of the ethical review processes</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1398,7 +1398,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Description of the process to access to raw data</t>
+          <t>Description of the dataset retention policy</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1438,27 +1438,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Description of the dataset retention policy</t>
+          <t>Dataset name</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1478,22 +1478,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Description of the confidential data</t>
+          <t>Details of the data modalities</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1518,7 +1518,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Description of the data sampling process</t>
+          <t>Description of the process to access to raw data</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1558,7 +1558,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Description of the ethical review processes</t>
+          <t>Description of the data cleaning process</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1598,12 +1598,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Version of the dataset associated with this dataset documentation</t>
+          <t>Description of the confidential data</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1638,12 +1638,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dataset name</t>
+          <t>Description of the upsetting data</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1653,17 +1653,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1678,7 +1678,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Description of how consent for data collection and use was requested and provided</t>
+          <t>Information about the creators of the dataset</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Description of the data cleaning process</t>
+          <t>Description of how consent for data collection and use was requested and provided</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1758,7 +1758,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Information about the people tasked with data labeling</t>
+          <t>Description of the changes between dataset versions</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1798,12 +1798,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Information about the managers of the dataset</t>
+          <t>Description of the correlations in the dataset</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1813,17 +1813,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1831,24 +1831,24 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Information about dataset audit/review</t>
+          <t>Information about the managers of the dataset</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1871,19 +1871,19 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Description of the data annotation process</t>
+          <t>Description of the compensation for people involved in data collection</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1893,17 +1893,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1911,19 +1911,19 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Citation requirements when using the dataset</t>
+          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1958,12 +1958,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Description of the correlations in the dataset</t>
+          <t>Information about the curators of the dataset</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1973,17 +1973,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1991,19 +1991,19 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Description of the people involved in data collection</t>
+          <t>Description of the data content</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2013,17 +2013,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -2038,12 +2038,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Description of the changes between dataset versions</t>
+          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2078,12 +2078,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Description of the data preprocessing process</t>
+          <t>Citation requirements when using the dataset</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -2118,7 +2118,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Description of the potential impact of the dataset on data subjects</t>
+          <t>Description of the external resources the dataset relies on</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Description of the data maintenance plan</t>
+          <t>Information about the authors of this dataset documentation</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2168,12 +2168,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Description of the external resources the dataset relies on</t>
+          <t>Description of how individuals involved were notified regarding collection of their data</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2238,17 +2238,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Details regarding the dataset's representativeness if it is a sample</t>
+          <t>Indication of whether dataset includes data from humans</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2278,7 +2278,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Description of the data content</t>
+          <t>Description of the data annotation process</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2318,12 +2318,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Description of the methods to contribute to the dataset</t>
+          <t>Information about the people tasked with data labeling</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2358,7 +2358,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Description of the compensation for people involved in data collection</t>
+          <t>Description of the recommended data splits</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2398,12 +2398,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Description of the elements that may impact future uses of the dataset</t>
+          <t>Description of the performance of the dataset</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2431,19 +2431,19 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Description of how individuals involved were notified regarding collection of their data</t>
+          <t>Description of the data maintenance plan</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2453,17 +2453,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2478,7 +2478,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
+          <t>Description of the management plan for older versions of the dataset</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2511,14 +2511,14 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
+          <t>Details regarding the dataset's representativeness if it is a sample</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2558,17 +2558,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Information about the authors of this dataset documentation</t>
+          <t>Description of the consent revocation mechanism</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2578,12 +2578,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2598,7 +2598,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Description of the recommended data splits</t>
+          <t>Description of the potential impact of the dataset on data subjects</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2638,17 +2638,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Description of who the dataset will be shared with</t>
+          <t>Information about dataset audit/review</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2671,14 +2671,14 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Description of the management plan for older versions of the dataset</t>
+          <t>Description of the methods to contribute to the dataset</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Indication of whether dataset includes data from humans</t>
+          <t>Description of the people involved in data collection</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Link to an erratum</t>
+          <t>Dataset size and other metrics</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2773,17 +2773,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -2791,14 +2791,14 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Information about the curators of the dataset</t>
+          <t>Description of who the dataset will be shared with</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Description of the consent revocation mechanism</t>
+          <t>Description of the data preprocessing process</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2878,12 +2878,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Dataset size</t>
+          <t>Link to an erratum</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2893,17 +2893,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2911,19 +2911,19 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Description of the performance of the dataset</t>
+          <t>Description of the elements that may impact future uses of the dataset</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2951,14 +2951,14 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Description of the confounding factors that might be present in the data</t>
+          <t>Description of issues related to this dataset</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2978,7 +2978,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2998,7 +2998,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Dataset maintenance status</t>
+          <t>Number of subjects represented in the dataset</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3018,12 +3018,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -3038,7 +3038,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Description of the human data attributes</t>
+          <t>Description and results of the adversarial testing</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -3078,7 +3078,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Description of the relevance of the data</t>
+          <t>Description of the data exclusion criteria</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -3111,14 +3111,14 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Description of the process to mitigate risk from sensitive data</t>
+          <t>Keywords</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -3158,7 +3158,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Description of the dimensionality reduction</t>
+          <t>Description of the accessibility measurements</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3178,12 +3178,12 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -3198,7 +3198,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Description of annotations</t>
+          <t>Link to requirements specification</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -3231,14 +3231,14 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Description of the data rating process</t>
+          <t>Description of other transformations</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -3278,7 +3278,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Description and handling of the outliers</t>
+          <t>Description of the confounding factors that might be present in the data</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3298,12 +3298,12 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -3318,7 +3318,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Information about risks when used with other data</t>
+          <t>Description of the strategies to avoid reidentification</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3338,12 +3338,12 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -3358,7 +3358,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>List of related documents</t>
+          <t>Guidelines for creating new labels</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3373,12 +3373,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3391,14 +3391,14 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Description of domain specific concepts for general readers</t>
+          <t>Last update date</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3431,14 +3431,14 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Description of representation issues in the data</t>
+          <t>Link to design document</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3448,12 +3448,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3471,14 +3471,14 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Description of the dataset processing process</t>
+          <t>Information about the people consulted to create this dataset documentation</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3488,12 +3488,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Information about the first version of the dataset</t>
+          <t>Description of representation issues in the data</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3528,7 +3528,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3551,14 +3551,14 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Description and results of other testing</t>
+          <t>Description of the prerequisites to access this dataset</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -3591,14 +3591,14 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid reidentification</t>
+          <t>Expectations for people using the dataset</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3631,14 +3631,14 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Keywords</t>
+          <t>Countries where the data was collected</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3671,14 +3671,14 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Expectations for people using the dataset</t>
+          <t>Description of the regulation preventing demographic data collection</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3693,12 +3693,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3711,14 +3711,14 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Number of subjects represented in the dataset</t>
+          <t>Description of annotations</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3738,12 +3738,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -3758,7 +3758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
+          <t>Description and handling of mismatched values</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3798,7 +3798,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Description of the joint inputs sourced</t>
+          <t>Description of the individual-level data</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3823,7 +3823,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -3831,14 +3831,14 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Description of the data quality measurements</t>
+          <t>Description of the ethical impact of the data and its collection</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Description of the redacted or anonymized features</t>
+          <t>Description of the relevance of the data</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G87" t="n">
@@ -3911,14 +3911,14 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Description of the process for creating this dataset documentation</t>
+          <t>Description of related datasets</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3951,14 +3951,14 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Information about the data collection cost</t>
+          <t>List of related documents</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Description of the data validation process</t>
+          <t>Information about the first version of the dataset</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4031,14 +4031,14 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Description and results of the adversarial testing</t>
+          <t>Description of the privacy handling</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -4071,14 +4071,14 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Recommendations when used in AI/ML systems</t>
+          <t>Information about the dataset versioning approach</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -4098,12 +4098,12 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -4111,14 +4111,14 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Description of the data selection and inclusion criteria</t>
+          <t>Description of domain specific concepts for general readers</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -4151,14 +4151,14 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Guidelines for creating new labels</t>
+          <t>Description of the joint inputs sourced</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -4178,12 +4178,12 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -4198,7 +4198,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Description of the privacy handling</t>
+          <t>Information about the data collection cost</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -4231,14 +4231,14 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Description of the ethical impact of the data and its collection</t>
+          <t>Description of the data validation process</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -4278,7 +4278,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Information about the dataset versioning approach</t>
+          <t>Description of the choice(s) of language for communication with study participants</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -4311,14 +4311,14 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Description of other transformations</t>
+          <t>Description of the human data attributes</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -4351,14 +4351,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Description of the dataset deletion process</t>
+          <t>Assumption in data fields not made explicit in the data dictionary</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -4398,7 +4398,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Recommendations when sampling the dataset</t>
+          <t>Description and results of other testing</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -4423,7 +4423,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -4431,14 +4431,14 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Description of the proxy characteristics in the dataset</t>
+          <t>Description of the data rating process</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -4448,12 +4448,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Description of the data exclusion criteria</t>
+          <t>Description and handling of the outliers</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -4518,7 +4518,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Description of what is being tested in the dataset</t>
+          <t>Recommendations when sampling the dataset</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4543,7 +4543,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -4558,7 +4558,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Information about the format/structure of the dataset</t>
+          <t>Information about the dataset documentation for other version of this dataset</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4591,14 +4591,14 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Assumption in data fields not made explicit in the data dictionary</t>
+          <t>Dataset maintenance status</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -4631,14 +4631,14 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Description of the involvement of the participants in the dataset planning/collection</t>
+          <t>Details of the data points</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -4671,14 +4671,14 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Recommendations when this data is used with other data</t>
+          <t>Information about the format/structure of the dataset</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -4688,7 +4688,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4703,7 +4703,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -4718,7 +4718,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Description of the accessibility measurements</t>
+          <t>Description of benefits of the dataset compared to upstream sources</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4738,12 +4738,12 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -4758,7 +4758,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Familiarity of creators of this dataset documentation with the dataset</t>
+          <t>Information about the metadata repository and data dictionary</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -4798,7 +4798,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Required domain-specific knowledge for proper use of the dataset</t>
+          <t>Description of the aggregated data</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -4808,7 +4808,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -4878,7 +4878,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Statistics about each data field</t>
+          <t>Description of the process for creating this dataset documentation</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G112" t="n">
@@ -4911,14 +4911,14 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Known issues with data collection</t>
+          <t>Description of the strategies to avoid undesired population-level inferences</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4958,7 +4958,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Known caveats about the dataset</t>
+          <t>Description of the process to mitigate risk from sensitive data</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -4991,14 +4991,14 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Information about the dataset documentation for other version of this dataset</t>
+          <t>Description of the study inclusion criteria</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -5031,14 +5031,14 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Information about the dataset publishers</t>
+          <t>Description of the redacted or anonymized features</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -5078,7 +5078,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Countries where the data was collected</t>
+          <t>Description of the dataset processing process</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -5093,12 +5093,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -5118,7 +5118,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Description of the aggregated data</t>
+          <t>Description of the dataset deletion process</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -5158,7 +5158,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Description of the alignment of the dataset with upstream sources</t>
+          <t>Description of the involvement of the participants in the dataset planning/collection</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G119" t="n">
@@ -5191,14 +5191,14 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Description of the prerequisites to access this dataset</t>
+          <t>Known issues with data collection</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -5208,7 +5208,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -5223,7 +5223,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G120" t="n">
@@ -5238,17 +5238,17 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Description of the possibilities to identify individuals from the data</t>
+          <t>Familiarity of creators of this dataset documentation with the dataset</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -5278,7 +5278,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Description of the data distribution in the dataset</t>
+          <t>Description of the proxy characteristics in the dataset</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -5288,12 +5288,12 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -5311,14 +5311,14 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Description of the study inclusion criteria</t>
+          <t>Description of the data distribution in the dataset</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -5333,12 +5333,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -5358,7 +5358,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Last update date</t>
+          <t>Description of the alignment of the dataset with upstream sources</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -5373,7 +5373,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -5398,7 +5398,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
+          <t>Statistics about each data field</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -5418,12 +5418,12 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -5431,14 +5431,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Description of related datasets</t>
+          <t>Information about risks when used with other data</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -5463,7 +5463,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -5471,14 +5471,14 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Details of the data points</t>
+          <t>Description of the dimensionality reduction</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -5511,14 +5511,14 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Description and results of the requirement testing</t>
+          <t>Known caveats about the dataset</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -5551,14 +5551,14 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Link to requirements specification</t>
+          <t>Description of what is being tested in the dataset</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -5591,14 +5591,14 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid undesired population-level inferences</t>
+          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -5638,7 +5638,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Description of the choice(s) of language for communication with study participants</t>
+          <t>Description of the data selection and inclusion criteria</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -5658,12 +5658,12 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -5678,7 +5678,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Information about the people consulted to create this dataset documentation</t>
+          <t>Recommendations when this data is used with other data</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -5718,7 +5718,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Description of the regulation preventing demographic data collection</t>
+          <t>Information about the dataset publishers</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -5738,12 +5738,12 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -5751,24 +5751,24 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Information about the metadata repository and data dictionary</t>
+          <t>Description of the possibilities to identify individuals from the data</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -5791,14 +5791,14 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Link to design document</t>
+          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -5823,7 +5823,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -5831,14 +5831,14 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Other dataset metrics besides size</t>
+          <t>Required domain-specific knowledge for proper use of the dataset</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -5871,14 +5871,14 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Description of benefits of the dataset compared to upstream sources</t>
+          <t>Recommendations when used in AI/ML systems</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -5911,14 +5911,14 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Description and handling of mismatched values</t>
+          <t>Description of the data quality measurements</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G138" t="n">
@@ -5958,7 +5958,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Description of issues related to this dataset</t>
+          <t>Description and results of the requirement testing</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -5968,12 +5968,12 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -5990,46 +5990,6 @@
         <v>1</v>
       </c>
       <c r="H139" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>Description of the individual-level data</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="G140" t="n">
-        <v>1</v>
-      </c>
-      <c r="H140" t="inlineStr">
         <is>
           <t>no</t>
         </is>

</xml_diff>

<commit_message>
fix: rerun real word doc analysis
</commit_message>
<xml_diff>
--- a/outputs/metadata_elements_count.xlsx
+++ b/outputs/metadata_elements_count.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Description of the data collection process</t>
+          <t>Dataset publication date</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Description of the intended use of the dataset</t>
+          <t>Information about the owners of the dataset</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -543,7 +543,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Information about the owners of the dataset</t>
+          <t>Description of the intended use of the dataset</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dataset publication date</t>
+          <t>Description of the dataset update plan</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -613,7 +613,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Description of the dataset update plan</t>
+          <t>Details about the funding of the dataset</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -648,7 +648,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Details about the funding of the dataset</t>
+          <t>Description of the data collection process</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Description of the purpose for creating the dataset</t>
+          <t>Description of the instances included in the dataset</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -728,7 +728,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -753,7 +753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Information about the maintainers of the dataset</t>
+          <t>Description of the data collection timeframe</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Description of the instances included in the dataset</t>
+          <t>Description of the purpose for creating the dataset</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -823,7 +823,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DOI or link of the dataset</t>
+          <t>Description of the restrictions on the usage of the data</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -928,7 +928,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Description of the data collection timeframe</t>
+          <t>Description of the dataset license and/or terms of use</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Description of the sensitive data</t>
+          <t>DOI or link of the dataset</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1033,7 +1033,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Description of the restrictions on the usage of the data</t>
+          <t>Description of the sensitive data</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1068,12 +1068,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Description of the dataset license and/or terms of use</t>
+          <t>Description of the dataset</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1138,12 +1138,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Description of the dataset</t>
+          <t>Information about the maintainers of the dataset</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1173,7 +1173,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Version of the dataset associated with this dataset documentation</t>
+          <t>Dataset name</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1188,12 +1188,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1208,22 +1208,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Description of the upsetting data</t>
+          <t>Details of the data modalities</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1243,7 +1243,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Description of the ethical review processes</t>
+          <t>Description of the process to access to raw data</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1278,22 +1278,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Details of the data modalities</t>
+          <t>Information about the creators of the dataset</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1313,7 +1313,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Information about the creators of the dataset</t>
+          <t>Description of the confidential data</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1348,17 +1348,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Description of the dataset retention policy</t>
+          <t>Version of the dataset associated with this dataset documentation</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1383,7 +1383,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Description of the data cleaning process</t>
+          <t>Description of the data sampling process</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1418,27 +1418,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Dataset name</t>
+          <t>Description of the dataset retention policy</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1453,7 +1453,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Description of the data sampling process</t>
+          <t>Description of how consent for data collection and use was requested and provided</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1488,7 +1488,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Description of how consent for data collection and use was requested and provided</t>
+          <t>Description of the data cleaning process</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1523,7 +1523,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Description of the process to access to raw data</t>
+          <t>Description of the ethical review processes</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Description of the confidential data</t>
+          <t>Description of the upsetting data</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1593,7 +1593,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Description of the data annotation process</t>
+          <t>Dataset size and other metrics</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Description of the correlations in the dataset</t>
+          <t>Information about the people tasked with data labeling</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1663,7 +1663,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
+          <t>Description of how individuals involved were notified regarding collection of their data</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1698,12 +1698,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Description of the consent revocation mechanism</t>
+          <t>Description of the performance of the dataset</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1733,7 +1733,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Indication of whether dataset includes data from humans</t>
+          <t>Citation requirements when using the dataset</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1768,7 +1768,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Description of the external resources the dataset relies on</t>
+          <t>Description of the potential impact of the dataset on data subjects</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1803,7 +1803,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Description of the data maintenance plan</t>
+          <t>Information about the authors of this dataset documentation</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1813,12 +1813,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Description of the compensation for people involved in data collection</t>
+          <t>Details regarding the dataset's representativeness if it is a sample</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1873,17 +1873,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Information about dataset audit/review</t>
+          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Description of the management plan for older versions of the dataset</t>
+          <t>Description of the data preprocessing process</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
+          <t>Description of the elements that may impact future uses of the dataset</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1978,7 +1978,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Dataset size and other metrics</t>
+          <t>Description of the data maintenance plan</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2013,7 +2013,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Information about the authors of this dataset documentation</t>
+          <t>Description of the data annotation process</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2083,12 +2083,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Information about the people tasked with data labeling</t>
+          <t>Description of the management plan for older versions of the dataset</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2118,17 +2118,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Description of the recommended data splits</t>
+          <t>Indication of whether dataset includes data from humans</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2153,12 +2153,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Citation requirements when using the dataset</t>
+          <t>Description of the compensation for people involved in data collection</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2188,7 +2188,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Description of the potential impact of the dataset on data subjects</t>
+          <t>Description of the recommended data splits</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2223,12 +2223,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Description of the performance of the dataset</t>
+          <t>Description of the consent revocation mechanism</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2258,17 +2258,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Link to an erratum</t>
+          <t>Information about dataset audit/review</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2293,7 +2293,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Description of the data preprocessing process</t>
+          <t>Description of the external resources the dataset relies on</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2328,7 +2328,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Information about the managers of the dataset</t>
+          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2363,7 +2363,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Description of the people involved in data collection</t>
+          <t>Description of who the dataset will be shared with</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2398,7 +2398,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Description of how individuals involved were notified regarding collection of their data</t>
+          <t>Information about the managers of the dataset</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2433,12 +2433,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Description of the data content</t>
+          <t>Description of the people involved in data collection</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2448,17 +2448,17 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2468,12 +2468,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Information about the curators of the dataset</t>
+          <t>Description of the correlations in the dataset</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2483,17 +2483,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -2503,7 +2503,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Description of who the dataset will be shared with</t>
+          <t>Link to an erratum</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2573,12 +2573,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Details regarding the dataset's representativeness if it is a sample</t>
+          <t>Description of the data content</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2588,17 +2588,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2608,7 +2608,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Description of the elements that may impact future uses of the dataset</t>
+          <t>Information about the curators of the dataset</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2643,7 +2643,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Number of subjects represented in the dataset</t>
+          <t>Description of the privacy handling</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2658,12 +2658,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Description and handling of mismatched values</t>
+          <t>Description of representation issues that might be reflected in the data</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -2713,7 +2713,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Description of the regulation preventing demographic data collection</t>
+          <t>Information about the metadata repository and data dictionary</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2748,7 +2748,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Known caveats about the dataset</t>
+          <t>Recommendations when used in AI/ML systems</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2763,7 +2763,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2783,7 +2783,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Description of the data rating process</t>
+          <t>Description of annotations</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2818,7 +2818,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Recommendations when sampling the dataset</t>
+          <t>List of related documents</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2853,7 +2853,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Information about the dataset publishers</t>
+          <t>Description of the accessibility measurements</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2873,12 +2873,12 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -2888,7 +2888,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Information about the format/structure of the dataset</t>
+          <t>Assumption in data fields not made explicit in the data dictionary</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2923,7 +2923,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Description of benefits of the dataset compared to upstream sources</t>
+          <t>Expectations for people using the dataset</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -2958,7 +2958,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Description of the prerequisites to access this dataset</t>
+          <t>Description of the relevance of the data</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -2993,7 +2993,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Keywords</t>
+          <t>Information about the first version of the dataset</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3003,7 +3003,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3018,7 +3018,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -3028,7 +3028,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Description of the dimensionality reduction</t>
+          <t>Recommendations when sampling the dataset</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3063,7 +3063,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Description of issues related to this dataset</t>
+          <t>Description of the data quality measurements</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3073,12 +3073,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Assumption in data fields not made explicit in the data dictionary</t>
+          <t>Countries where the data was collected</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3133,7 +3133,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Description and results of other testing</t>
+          <t>Description of the alignment of the dataset with upstream sources</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3168,7 +3168,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Description of the dataset processing process</t>
+          <t>Description of the individual-level data</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3178,12 +3178,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3203,7 +3203,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Description and results of the requirement testing</t>
+          <t>Description and handling of mismatched values</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -3238,7 +3238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Description of the involvement of the participants in the dataset planning/collection</t>
+          <t>Information about the dataset versioning approach</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3273,7 +3273,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Description of the process for creating this dataset documentation</t>
+          <t>Information about the format/structure of the dataset</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3283,12 +3283,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Description of the data distribution in the dataset</t>
+          <t>Number of subjects represented in the dataset</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3323,12 +3323,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3343,7 +3343,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Information about the first version of the dataset</t>
+          <t>Description of the regulation preventing demographic data collection</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3363,12 +3363,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -3378,12 +3378,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Description of the data selection and inclusion criteria</t>
+          <t>Description of the possibilities to identify individuals from the data</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -3413,7 +3413,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Description of the data quality measurements</t>
+          <t>Information about risks when used with other data</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3438,7 +3438,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -3448,7 +3448,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Description of the proxy characteristics in the dataset</t>
+          <t>Recommendations when this data is used with other data</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G87" t="n">
@@ -3483,7 +3483,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Description of the accessibility measurements</t>
+          <t>Description of the ethical impact of the data and its collection</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3498,12 +3498,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Recommendations when this data is used with other data</t>
+          <t>Known issues with data collection</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3528,7 +3528,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G89" t="n">
@@ -3553,7 +3553,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Link to design document</t>
+          <t>Description of the choice(s) of language for communication with study participants</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3568,12 +3568,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3623,7 +3623,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Information about the data collection cost</t>
+          <t>Description of the involvement of the participants in the dataset planning/collection</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3633,12 +3633,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3658,7 +3658,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Required domain-specific knowledge for proper use of the dataset</t>
+          <t>Description of the proxy characteristics in the dataset</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3693,7 +3693,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Information about the metadata repository and data dictionary</t>
+          <t>Description and results of the requirement testing</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3703,12 +3703,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Description and results of the adversarial testing</t>
+          <t>Description of related datasets</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3763,7 +3763,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Description of representation issues that might be reflected in the data</t>
+          <t>Description of the data selection and inclusion criteria</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -3798,7 +3798,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
+          <t>Description of the strategies to avoid reidentification</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3818,12 +3818,12 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -3833,7 +3833,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Description of the aggregated data</t>
+          <t>Link to requirements specification</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -3868,7 +3868,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Recommendations when used in AI/ML systems</t>
+          <t>Description of the prerequisites to access this dataset</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3903,7 +3903,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>List of related documents</t>
+          <t>Information about the dataset publishers</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -3938,7 +3938,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Description of the dataset deletion process</t>
+          <t>Description of the dataset processing process</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G101" t="n">
@@ -3973,7 +3973,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Dataset maintenance status</t>
+          <t>Description of the aggregated data</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -4008,7 +4008,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Information about the dataset documentation for other version of this dataset</t>
+          <t>Description of benefits of the dataset compared to upstream sources</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4028,12 +4028,12 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -4043,7 +4043,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Description of the data validation process</t>
+          <t>Description of the redacted or anonymized features</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Familiarity of creators of this dataset documentation with the dataset</t>
+          <t>Dataset maintenance status</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -4113,7 +4113,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Description of the study inclusion criteria</t>
+          <t>Last update date</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4128,12 +4128,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Known issues with data collection</t>
+          <t>Description of the data distribution in the dataset</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -4158,12 +4158,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -4183,7 +4183,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Description of the data exclusion criteria</t>
+          <t>Information about the people consulted to create this dataset documentation</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -4218,7 +4218,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Description of annotations</t>
+          <t>Required domain-specific knowledge for proper use of the dataset</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4243,7 +4243,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G109" t="n">
@@ -4253,7 +4253,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Information about the people consulted to create this dataset documentation</t>
+          <t>Description of the joint inputs sourced</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -4288,7 +4288,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Description of other transformations</t>
+          <t>Description of what is being tested in the dataset</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -4303,7 +4303,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -4323,7 +4323,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Description of the privacy handling</t>
+          <t>Description of the data rating process</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Statistics about each data field</t>
+          <t>Description of the data validation process</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4393,7 +4393,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid reidentification</t>
+          <t>Known caveats about the dataset</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4428,7 +4428,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Description of the individual-level data</t>
+          <t>Description of the strategies to avoid undesired population-level inferences</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -4463,7 +4463,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Link to requirements specification</t>
+          <t>Statistics about each data field</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G116" t="n">
@@ -4533,7 +4533,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Description of related datasets</t>
+          <t>Description of the data exclusion criteria</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G118" t="n">
@@ -4568,7 +4568,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Last update date</t>
+          <t>Description of the process for creating this dataset documentation</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -4603,7 +4603,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
+          <t>Information about the dataset documentation for other version of this dataset</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -4638,7 +4638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Information about the dataset versioning approach</t>
+          <t>Description of other transformations</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -4658,12 +4658,12 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G121" t="n">
@@ -4673,7 +4673,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Description of the choice(s) of language for communication with study participants</t>
+          <t>Description of the confounding factors that might be present in the data</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -4708,7 +4708,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Description of the confounding factors that might be present in the data</t>
+          <t>Description of the dimensionality reduction</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -4728,12 +4728,12 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -4743,7 +4743,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Description and handling of the outliers</t>
+          <t>Details of the data points</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -4778,7 +4778,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Countries where the data was collected</t>
+          <t>Description and results of the adversarial testing</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4793,12 +4793,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -4813,7 +4813,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Description of the joint inputs sourced</t>
+          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -4848,7 +4848,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Expectations for people using the dataset</t>
+          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -4863,12 +4863,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4883,7 +4883,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Description of the redacted or anonymized features</t>
+          <t>Description of issues related to this dataset</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4908,7 +4908,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -4918,7 +4918,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Description of the ethical impact of the data and its collection</t>
+          <t>Description of the dataset deletion process</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G129" t="n">
@@ -4953,7 +4953,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Description of the process to mitigate risk from sensitive data</t>
+          <t>Description and results of other testing</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -4978,7 +4978,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G130" t="n">
@@ -4988,7 +4988,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Description of the relevance of the data</t>
+          <t>Description of the process to mitigate risk from sensitive data</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -5003,7 +5003,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -5023,7 +5023,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Description of the alignment of the dataset with upstream sources</t>
+          <t>Description and handling of the outliers</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -5093,7 +5093,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Details of the data points</t>
+          <t>Description of the study inclusion criteria</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -5113,12 +5113,12 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -5128,7 +5128,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Description of domain specific concepts for general readers</t>
+          <t>Information about the data collection cost</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -5163,12 +5163,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Description of the possibilities to identify individuals from the data</t>
+          <t>Link to design document</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5198,7 +5198,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid undesired population-level inferences</t>
+          <t>Keywords</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -5233,7 +5233,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Information about risks when used with other data</t>
+          <t>Description of domain specific concepts for general readers</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G138" t="n">
@@ -5268,7 +5268,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Description of what is being tested in the dataset</t>
+          <t>Familiarity of creators of this dataset documentation with the dataset</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -5278,12 +5278,12 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">

</xml_diff>

<commit_message>
fix: all code reviewed
</commit_message>
<xml_diff>
--- a/outputs/metadata_elements_count.xlsx
+++ b/outputs/metadata_elements_count.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dataset publication date</t>
+          <t>Description of the dataset sharing method</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Information about the owners of the dataset</t>
+          <t>Dataset publication date</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -543,7 +543,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Description of the intended use of the dataset</t>
+          <t>Description of the data collection process</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Description of the dataset update plan</t>
+          <t>Description of the intended use of the dataset</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -648,7 +648,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Description of the data collection process</t>
+          <t>Information about the owners of the dataset</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -683,7 +683,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Description of the dataset sharing method</t>
+          <t>Description of the dataset update plan</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Description of the instances included in the dataset</t>
+          <t>Description of the sensitive data</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -753,7 +753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Description of the data collection timeframe</t>
+          <t>Description of the dataset license and/or terms of use</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Description of the purpose for creating the dataset</t>
+          <t>Description of the instances included in the dataset</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -823,12 +823,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Description of the restrictions on the usage of the data</t>
+          <t>Description of the dataset</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -858,7 +858,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Description of the subpopulations identified in the dataset</t>
+          <t>DOI or link of the dataset</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -868,7 +868,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -893,7 +893,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Description and handling of the missing data</t>
+          <t>Description of the restrictions on the usage of the data</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -918,7 +918,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -928,7 +928,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Description of the dataset license and/or terms of use</t>
+          <t>Description of the data labeling process</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DOI or link of the dataset</t>
+          <t>Description and handling of the missing data</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Description of the undesirable uses of the dataset</t>
+          <t>Description of the subpopulations identified in the dataset</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1033,7 +1033,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Description of the sensitive data</t>
+          <t>Description of the undesirable uses of the dataset</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1043,12 +1043,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1068,12 +1068,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Description of the dataset</t>
+          <t>Description of the data collection timeframe</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1103,7 +1103,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Description of the data labeling process</t>
+          <t>Information about the maintainers of the dataset</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1138,7 +1138,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Information about the maintainers of the dataset</t>
+          <t>Description of the purpose for creating the dataset</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1173,12 +1173,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dataset name</t>
+          <t>Information about the creators of the dataset</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1188,17 +1188,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1208,22 +1208,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Details of the data modalities</t>
+          <t>Description of the upsetting data</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1278,7 +1278,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Information about the creators of the dataset</t>
+          <t>Description of the ethical review processes</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1313,7 +1313,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Description of the confidential data</t>
+          <t>Description of the data cleaning process</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1348,12 +1348,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Version of the dataset associated with this dataset documentation</t>
+          <t>Description of how consent for data collection and use was requested and provided</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1418,7 +1418,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Description of the dataset retention policy</t>
+          <t>Description of the confidential data</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1453,12 +1453,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Description of how consent for data collection and use was requested and provided</t>
+          <t>Version of the dataset associated with this dataset documentation</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1488,12 +1488,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Description of the data cleaning process</t>
+          <t>Dataset name</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1503,17 +1503,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1523,22 +1523,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Description of the ethical review processes</t>
+          <t>Details of the data modalities</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1558,7 +1558,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Description of the upsetting data</t>
+          <t>Description of the dataset retention policy</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1628,7 +1628,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Information about the people tasked with data labeling</t>
+          <t>Description of the data content</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1663,7 +1663,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Description of how individuals involved were notified regarding collection of their data</t>
+          <t>Description of the elements that may impact future uses of the dataset</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1698,7 +1698,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Description of the performance of the dataset</t>
+          <t>Information about the authors of this dataset documentation</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1708,22 +1708,22 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1733,7 +1733,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Citation requirements when using the dataset</t>
+          <t>Description of the changes between dataset versions</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1768,7 +1768,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Description of the potential impact of the dataset on data subjects</t>
+          <t>Information about the managers of the dataset</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1803,17 +1803,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Information about the authors of this dataset documentation</t>
+          <t>Description of the external resources the dataset relies on</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1823,12 +1823,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1838,7 +1838,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Details regarding the dataset's representativeness if it is a sample</t>
+          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1873,7 +1873,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Indication of whether the data was collected directly from individuals or from third party sources</t>
+          <t>Description of the management plan for older versions of the dataset</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Description of the data preprocessing process</t>
+          <t>Information about the curators of the dataset</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Description of the elements that may impact future uses of the dataset</t>
+          <t>Description of the data preprocessing process</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1978,7 +1978,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Description of the data maintenance plan</t>
+          <t>Information about dataset audit/review</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1988,22 +1988,22 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2013,12 +2013,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Description of the data annotation process</t>
+          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2028,17 +2028,17 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2048,7 +2048,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Description of the changes between dataset versions</t>
+          <t>Citation requirements when using the dataset</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2083,12 +2083,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Description of the management plan for older versions of the dataset</t>
+          <t>Description of the correlations in the dataset</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2098,17 +2098,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2118,17 +2118,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Indication of whether dataset includes data from humans</t>
+          <t>Details regarding the dataset's representativeness if it is a sample</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2153,7 +2153,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Description of the compensation for people involved in data collection</t>
+          <t>Description of the consent revocation mechanism</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Description of the recommended data splits</t>
+          <t>Description of the performance of the dataset</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2223,7 +2223,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Description of the consent revocation mechanism</t>
+          <t>Description of who the dataset will be shared with</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2258,17 +2258,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Information about dataset audit/review</t>
+          <t>Description of the people involved in data collection</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2293,7 +2293,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Description of the external resources the dataset relies on</t>
+          <t>Link to an erratum</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2328,7 +2328,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Description of the errors, sources or noises, and redundancies in the dataset</t>
+          <t>Description of the potential impact of the dataset on data subjects</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2363,7 +2363,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Description of who the dataset will be shared with</t>
+          <t>Description of how individuals involved were notified regarding collection of their data</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2398,7 +2398,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Information about the managers of the dataset</t>
+          <t>Description of the methods to contribute to the dataset</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2433,17 +2433,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Description of the people involved in data collection</t>
+          <t>Indication of whether dataset includes data from humans</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Description of the correlations in the dataset</t>
+          <t>Description of the data maintenance plan</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2503,12 +2503,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Link to an erratum</t>
+          <t>Description of the data annotation process</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2518,17 +2518,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -2538,12 +2538,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Description of the methods to contribute to the dataset</t>
+          <t>Information about the people tasked with data labeling</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2573,12 +2573,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Description of the data content</t>
+          <t>Description of the compensation for people involved in data collection</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2588,17 +2588,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2608,7 +2608,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Information about the curators of the dataset</t>
+          <t>Description of the recommended data splits</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2643,7 +2643,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Description of the privacy handling</t>
+          <t>Information about the dataset documentation for other version of this dataset</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2658,12 +2658,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Description of representation issues that might be reflected in the data</t>
+          <t>Familiarity of creators of this dataset documentation with the dataset</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2713,7 +2713,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Information about the metadata repository and data dictionary</t>
+          <t>Description of the data distribution in the dataset</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2723,12 +2723,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2748,7 +2748,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Recommendations when used in AI/ML systems</t>
+          <t>Description of domain specific concepts for general readers</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2763,7 +2763,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2783,7 +2783,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Description of annotations</t>
+          <t>Description of benefits of the dataset compared to upstream sources</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2818,7 +2818,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>List of related documents</t>
+          <t>Description of the dataset deletion process</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2853,7 +2853,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Description of the accessibility measurements</t>
+          <t>Description of the proxy characteristics in the dataset</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Assumption in data fields not made explicit in the data dictionary</t>
+          <t>Description of the confounding factors that might be present in the data</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2923,7 +2923,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Expectations for people using the dataset</t>
+          <t>Description of the data validation process</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -2958,7 +2958,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Description of the relevance of the data</t>
+          <t>Description of the choice(s) of language for communication with study participants</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2973,12 +2973,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3028,7 +3028,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Recommendations when sampling the dataset</t>
+          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -3063,7 +3063,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Description of the data quality measurements</t>
+          <t>Description of the redacted or anonymized features</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -3098,7 +3098,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Countries where the data was collected</t>
+          <t>Description of the dimensionality reduction</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3118,12 +3118,12 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -3133,7 +3133,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Description of the alignment of the dataset with upstream sources</t>
+          <t>Description of related datasets</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3168,7 +3168,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Description of the individual-level data</t>
+          <t>Description and results of the adversarial testing</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3178,12 +3178,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3203,7 +3203,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Description and handling of mismatched values</t>
+          <t>Description of the data rating process</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -3238,7 +3238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Information about the dataset versioning approach</t>
+          <t>Assumption in data fields not made explicit in the data dictionary</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3273,7 +3273,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Information about the format/structure of the dataset</t>
+          <t>Description of the accessibility measurements</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Number of subjects represented in the dataset</t>
+          <t>Description of the regulation preventing demographic data collection</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3343,7 +3343,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Description of the regulation preventing demographic data collection</t>
+          <t>Recommendations when sampling the dataset</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3363,12 +3363,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -3378,12 +3378,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Description of the possibilities to identify individuals from the data</t>
+          <t>Description and handling of the outliers</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -3413,7 +3413,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Information about risks when used with other data</t>
+          <t>Link to design document</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3438,7 +3438,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -3448,7 +3448,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Recommendations when this data is used with other data</t>
+          <t>Recommendations when used in AI/ML systems</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3483,7 +3483,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Description of the ethical impact of the data and its collection</t>
+          <t>Description of the data selection and inclusion criteria</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G88" t="n">
@@ -3518,7 +3518,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Known issues with data collection</t>
+          <t>Number of subjects represented in the dataset</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3528,7 +3528,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3553,7 +3553,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Description of the choice(s) of language for communication with study participants</t>
+          <t>Countries where the data was collected</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3588,7 +3588,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Description of limitations of the dataset compared to upstream sources</t>
+          <t>Description of the strategies to avoid reidentification</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3608,12 +3608,12 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -3623,7 +3623,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Description of the involvement of the participants in the dataset planning/collection</t>
+          <t>Information about the data collection cost</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3633,12 +3633,12 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3658,7 +3658,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Description of the proxy characteristics in the dataset</t>
+          <t>Description and results of the requirement testing</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3668,12 +3668,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3693,7 +3693,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Description and results of the requirement testing</t>
+          <t>Description of annotations</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3728,7 +3728,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Description of related datasets</t>
+          <t>Information about the dataset publishers</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -3763,7 +3763,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Description of the data selection and inclusion criteria</t>
+          <t>Description of the process for creating this dataset documentation</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3778,7 +3778,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -3798,7 +3798,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid reidentification</t>
+          <t>Information about the metadata repository and data dictionary</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3833,7 +3833,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Link to requirements specification</t>
+          <t>Dataset maintenance status</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -3868,7 +3868,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Description of the prerequisites to access this dataset</t>
+          <t>Known issues with data collection</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3878,7 +3878,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -3903,7 +3903,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Information about the dataset publishers</t>
+          <t>Description of the alignment of the dataset with upstream sources</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Description of the dataset processing process</t>
+          <t>Required domain-specific knowledge for proper use of the dataset</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3948,12 +3948,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3973,7 +3973,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Description of the aggregated data</t>
+          <t>Description of the individual-level data</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -4008,7 +4008,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Description of benefits of the dataset compared to upstream sources</t>
+          <t>Description of the privacy handling</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -4043,7 +4043,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Description of the redacted or anonymized features</t>
+          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Dataset maintenance status</t>
+          <t>Description of the data quality measurements</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -4093,7 +4093,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -4113,7 +4113,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Last update date</t>
+          <t>Known caveats about the dataset</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Description of the data distribution in the dataset</t>
+          <t>Description of the aggregated data</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -4183,7 +4183,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Information about the people consulted to create this dataset documentation</t>
+          <t>Description of representation issues that might be reflected in the data</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4218,7 +4218,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Required domain-specific knowledge for proper use of the dataset</t>
+          <t>Description of the strategies to avoid undesired population-level inferences</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -4253,7 +4253,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Description of the joint inputs sourced</t>
+          <t>Expectations for people using the dataset</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -4288,7 +4288,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Description of what is being tested in the dataset</t>
+          <t>Description and handling of mismatched values</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -4303,7 +4303,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -4323,7 +4323,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Description of the data rating process</t>
+          <t>Description of the involvement of the participants in the dataset planning/collection</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -4333,12 +4333,12 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Description of the data validation process</t>
+          <t>Description of the study inclusion criteria</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4378,12 +4378,12 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G113" t="n">
@@ -4393,7 +4393,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Known caveats about the dataset</t>
+          <t>Description of the data exclusion criteria</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -4408,7 +4408,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -4428,7 +4428,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Description of the strategies to avoid undesired population-level inferences</t>
+          <t>Information about the people consulted to create this dataset documentation</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -4463,7 +4463,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Statistics about each data field</t>
+          <t>Details of the data points</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Guidelines for creating new labels</t>
+          <t>Description of the joint inputs sourced</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -4518,12 +4518,12 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G117" t="n">
@@ -4533,7 +4533,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Description of the data exclusion criteria</t>
+          <t>Description of limitations of the dataset compared to upstream sources</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Description of the process for creating this dataset documentation</t>
+          <t>Information about the dataset versioning approach</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -4583,12 +4583,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -4603,7 +4603,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Information about the dataset documentation for other version of this dataset</t>
+          <t>Description of other transformations</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -4623,12 +4623,12 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G120" t="n">
@@ -4638,7 +4638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Description of other transformations</t>
+          <t>Keywords</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G121" t="n">
@@ -4673,7 +4673,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Description of the confounding factors that might be present in the data</t>
+          <t>Description of the process to mitigate risk from sensitive data</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -4693,12 +4693,12 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -4708,7 +4708,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Description of the dimensionality reduction</t>
+          <t>Statistics about each data field</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -4743,12 +4743,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Details of the data points</t>
+          <t>Description of the possibilities to identify individuals from the data</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -4778,7 +4778,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Description and results of the adversarial testing</t>
+          <t>Link to requirements specification</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4813,7 +4813,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Definition of the acronyms and concepts used in this dataset documentation</t>
+          <t>Description of the relevance of the data</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -4848,7 +4848,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Description of the factors in the data that might limit generalization of potentially derived model</t>
+          <t>Information about the format/structure of the dataset</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4883,7 +4883,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Description of issues related to this dataset</t>
+          <t>Description of what is being tested in the dataset</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -4893,12 +4893,12 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -4918,7 +4918,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Description of the dataset deletion process</t>
+          <t>Recommendations when this data is used with other data</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -4953,7 +4953,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Description and results of other testing</t>
+          <t>Description of the ethical impact of the data and its collection</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Description of the process to mitigate risk from sensitive data</t>
+          <t>Information about risks when used with other data</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -5023,7 +5023,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Description and handling of the outliers</t>
+          <t>Last update date</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -5048,7 +5048,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -5058,7 +5058,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Description of the human data attributes</t>
+          <t>Description of the dataset processing process</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -5093,7 +5093,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Description of the study inclusion criteria</t>
+          <t>Description of issues related to this dataset</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Information about the data collection cost</t>
+          <t>Guidelines for creating new labels</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -5143,12 +5143,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -5163,7 +5163,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Link to design document</t>
+          <t>Description of the prerequisites to access this dataset</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5188,7 +5188,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -5198,7 +5198,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Keywords</t>
+          <t>List of related documents</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -5208,12 +5208,12 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -5233,7 +5233,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Description of domain specific concepts for general readers</t>
+          <t>Description and results of other testing</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -5268,7 +5268,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Familiarity of creators of this dataset documentation with the dataset</t>
+          <t>Description of the human data attributes</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -5293,7 +5293,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G139" t="n">

</xml_diff>